<commit_message>
change templates per stampa in una pagina gestione tasto modifica per interventi esistenti (derivato da implementazione prodotti aggiuntivi)
</commit_message>
<xml_diff>
--- a/src/assets/template_riparazione.xlsx
+++ b/src/assets/template_riparazione.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr filterPrivacy="1" codeName="Questa_cartella_di_lavoro"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30482819-1638-924D-9F48-BD3729A2F129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CB72C2-F6CD-A54F-955D-4573D9BAE2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RICEVUTA" sheetId="5" r:id="rId1"/>
     <sheet name="Foglio3" sheetId="6" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">RICEVUTA!$A$1:$L$79</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">RICEVUTA!$B$1:$K$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1259,6 +1259,9 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1286,35 +1289,32 @@
     <xf numFmtId="0" fontId="33" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -1966,8 +1966,8 @@
   </sheetPr>
   <dimension ref="B1:K75"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B70" sqref="B1:K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2024,7 +2024,7 @@
       <c r="C5" s="34"/>
       <c r="D5" s="21"/>
       <c r="E5" s="68"/>
-      <c r="F5" s="72"/>
+      <c r="F5" s="73"/>
     </row>
     <row r="6" spans="2:11" s="9" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="34" t="s">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="C6" s="34"/>
       <c r="D6" s="21"/>
-      <c r="F6" s="72"/>
+      <c r="F6" s="73"/>
     </row>
     <row r="7" spans="2:11" s="9" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="34" t="s">
@@ -2055,10 +2055,10 @@
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="2:11" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="78"/>
+      <c r="C10" s="79"/>
       <c r="D10" s="38" t="s">
         <v>9</v>
       </c>
@@ -2070,8 +2070,8 @@
       </c>
     </row>
     <row r="11" spans="2:11" s="4" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="73"/>
-      <c r="C11" s="74"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="75"/>
       <c r="D11" s="65"/>
       <c r="E11" s="67"/>
       <c r="F11" s="40"/>
@@ -2081,22 +2081,22 @@
       <c r="K11" s="35"/>
     </row>
     <row r="12" spans="2:11" s="4" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="73"/>
-      <c r="C12" s="74"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="45"/>
       <c r="E12" s="46"/>
       <c r="F12" s="41"/>
     </row>
     <row r="13" spans="2:11" s="4" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="73"/>
-      <c r="C13" s="74"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="75"/>
       <c r="D13" s="44"/>
       <c r="E13" s="66"/>
       <c r="F13" s="40"/>
     </row>
     <row r="14" spans="2:11" s="4" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="75"/>
-      <c r="C14" s="76"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="77"/>
       <c r="D14" s="47"/>
       <c r="E14" s="62"/>
       <c r="F14" s="42"/>
@@ -2167,17 +2167,17 @@
       </c>
     </row>
     <row r="21" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="71" t="s">
+      <c r="B21" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="71"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="71"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="72"/>
     </row>
     <row r="22" spans="2:11" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="7"/>
@@ -2189,7 +2189,7 @@
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
       <c r="D23" s="56"/>
-      <c r="F23" s="70"/>
+      <c r="F23" s="71"/>
     </row>
     <row r="24" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="12" t="str">
@@ -2199,7 +2199,7 @@
       <c r="C24" s="12"/>
       <c r="D24" s="60"/>
       <c r="E24" s="54"/>
-      <c r="F24" s="70"/>
+      <c r="F24" s="71"/>
     </row>
     <row r="25" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="12" t="str">
@@ -2252,358 +2252,358 @@
       <c r="D30" s="26"/>
     </row>
     <row r="31" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="81" t="s">
+      <c r="B31" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="81"/>
-      <c r="D31" s="81"/>
-      <c r="E31" s="81"/>
-      <c r="F31" s="81"/>
-      <c r="G31" s="81"/>
-      <c r="H31" s="81"/>
-      <c r="I31" s="81"/>
-      <c r="J31" s="81"/>
-      <c r="K31" s="81"/>
+      <c r="C31" s="84"/>
+      <c r="D31" s="84"/>
+      <c r="E31" s="84"/>
+      <c r="F31" s="84"/>
+      <c r="G31" s="84"/>
+      <c r="H31" s="84"/>
+      <c r="I31" s="84"/>
+      <c r="J31" s="84"/>
+      <c r="K31" s="84"/>
     </row>
     <row r="32" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B32" s="81"/>
-      <c r="C32" s="81"/>
-      <c r="D32" s="81"/>
-      <c r="E32" s="81"/>
-      <c r="F32" s="81"/>
-      <c r="G32" s="81"/>
-      <c r="H32" s="81"/>
-      <c r="I32" s="81"/>
-      <c r="J32" s="81"/>
-      <c r="K32" s="81"/>
+      <c r="B32" s="84"/>
+      <c r="C32" s="84"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="84"/>
+      <c r="F32" s="84"/>
+      <c r="G32" s="84"/>
+      <c r="H32" s="84"/>
+      <c r="I32" s="84"/>
+      <c r="J32" s="84"/>
+      <c r="K32" s="84"/>
     </row>
     <row r="33" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="81"/>
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="81"/>
-      <c r="G33" s="81"/>
-      <c r="H33" s="81"/>
-      <c r="I33" s="81"/>
-      <c r="J33" s="81"/>
-      <c r="K33" s="81"/>
+      <c r="B33" s="84"/>
+      <c r="C33" s="84"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="84"/>
+      <c r="F33" s="84"/>
+      <c r="G33" s="84"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="84"/>
+      <c r="J33" s="84"/>
+      <c r="K33" s="84"/>
     </row>
     <row r="34" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="81"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="81"/>
-      <c r="G34" s="81"/>
-      <c r="H34" s="81"/>
-      <c r="I34" s="81"/>
-      <c r="J34" s="81"/>
-      <c r="K34" s="81"/>
+      <c r="B34" s="84"/>
+      <c r="C34" s="84"/>
+      <c r="D34" s="84"/>
+      <c r="E34" s="84"/>
+      <c r="F34" s="84"/>
+      <c r="G34" s="84"/>
+      <c r="H34" s="84"/>
+      <c r="I34" s="84"/>
+      <c r="J34" s="84"/>
+      <c r="K34" s="84"/>
     </row>
     <row r="35" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B35" s="81"/>
-      <c r="C35" s="81"/>
-      <c r="D35" s="81"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="81"/>
-      <c r="G35" s="81"/>
-      <c r="H35" s="81"/>
-      <c r="I35" s="81"/>
-      <c r="J35" s="81"/>
-      <c r="K35" s="81"/>
+      <c r="B35" s="84"/>
+      <c r="C35" s="84"/>
+      <c r="D35" s="84"/>
+      <c r="E35" s="84"/>
+      <c r="F35" s="84"/>
+      <c r="G35" s="84"/>
+      <c r="H35" s="84"/>
+      <c r="I35" s="84"/>
+      <c r="J35" s="84"/>
+      <c r="K35" s="84"/>
     </row>
     <row r="36" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="81"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
-      <c r="G36" s="81"/>
-      <c r="H36" s="81"/>
-      <c r="I36" s="81"/>
-      <c r="J36" s="81"/>
-      <c r="K36" s="81"/>
+      <c r="B36" s="84"/>
+      <c r="C36" s="84"/>
+      <c r="D36" s="84"/>
+      <c r="E36" s="84"/>
+      <c r="F36" s="84"/>
+      <c r="G36" s="84"/>
+      <c r="H36" s="84"/>
+      <c r="I36" s="84"/>
+      <c r="J36" s="84"/>
+      <c r="K36" s="84"/>
     </row>
     <row r="37" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="81"/>
-      <c r="C37" s="81"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
-      <c r="G37" s="81"/>
-      <c r="H37" s="81"/>
-      <c r="I37" s="81"/>
-      <c r="J37" s="81"/>
-      <c r="K37" s="81"/>
+      <c r="B37" s="84"/>
+      <c r="C37" s="84"/>
+      <c r="D37" s="84"/>
+      <c r="E37" s="84"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="84"/>
+      <c r="H37" s="84"/>
+      <c r="I37" s="84"/>
+      <c r="J37" s="84"/>
+      <c r="K37" s="84"/>
     </row>
     <row r="38" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B38" s="81"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="81"/>
-      <c r="E38" s="81"/>
-      <c r="F38" s="81"/>
-      <c r="G38" s="81"/>
-      <c r="H38" s="81"/>
-      <c r="I38" s="81"/>
-      <c r="J38" s="81"/>
-      <c r="K38" s="81"/>
+      <c r="B38" s="84"/>
+      <c r="C38" s="84"/>
+      <c r="D38" s="84"/>
+      <c r="E38" s="84"/>
+      <c r="F38" s="84"/>
+      <c r="G38" s="84"/>
+      <c r="H38" s="84"/>
+      <c r="I38" s="84"/>
+      <c r="J38" s="84"/>
+      <c r="K38" s="84"/>
     </row>
     <row r="39" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B39" s="81"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
-      <c r="G39" s="81"/>
-      <c r="H39" s="81"/>
-      <c r="I39" s="81"/>
-      <c r="J39" s="81"/>
-      <c r="K39" s="81"/>
+      <c r="B39" s="84"/>
+      <c r="C39" s="84"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="84"/>
+      <c r="F39" s="84"/>
+      <c r="G39" s="84"/>
+      <c r="H39" s="84"/>
+      <c r="I39" s="84"/>
+      <c r="J39" s="84"/>
+      <c r="K39" s="84"/>
     </row>
     <row r="40" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B40" s="81"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="81"/>
-      <c r="G40" s="81"/>
-      <c r="H40" s="81"/>
-      <c r="I40" s="81"/>
-      <c r="J40" s="81"/>
-      <c r="K40" s="81"/>
+      <c r="B40" s="84"/>
+      <c r="C40" s="84"/>
+      <c r="D40" s="84"/>
+      <c r="E40" s="84"/>
+      <c r="F40" s="84"/>
+      <c r="G40" s="84"/>
+      <c r="H40" s="84"/>
+      <c r="I40" s="84"/>
+      <c r="J40" s="84"/>
+      <c r="K40" s="84"/>
     </row>
     <row r="41" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B41" s="81"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="81"/>
-      <c r="F41" s="81"/>
-      <c r="G41" s="81"/>
-      <c r="H41" s="81"/>
-      <c r="I41" s="81"/>
-      <c r="J41" s="81"/>
-      <c r="K41" s="81"/>
+      <c r="B41" s="84"/>
+      <c r="C41" s="84"/>
+      <c r="D41" s="84"/>
+      <c r="E41" s="84"/>
+      <c r="F41" s="84"/>
+      <c r="G41" s="84"/>
+      <c r="H41" s="84"/>
+      <c r="I41" s="84"/>
+      <c r="J41" s="84"/>
+      <c r="K41" s="84"/>
     </row>
     <row r="42" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B42" s="81"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="81"/>
-      <c r="F42" s="81"/>
-      <c r="G42" s="81"/>
-      <c r="H42" s="81"/>
-      <c r="I42" s="81"/>
-      <c r="J42" s="81"/>
-      <c r="K42" s="81"/>
+      <c r="B42" s="84"/>
+      <c r="C42" s="84"/>
+      <c r="D42" s="84"/>
+      <c r="E42" s="84"/>
+      <c r="F42" s="84"/>
+      <c r="G42" s="84"/>
+      <c r="H42" s="84"/>
+      <c r="I42" s="84"/>
+      <c r="J42" s="84"/>
+      <c r="K42" s="84"/>
     </row>
     <row r="43" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B43" s="81"/>
-      <c r="C43" s="81"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="81"/>
-      <c r="G43" s="81"/>
-      <c r="H43" s="81"/>
-      <c r="I43" s="81"/>
-      <c r="J43" s="81"/>
-      <c r="K43" s="81"/>
+      <c r="B43" s="84"/>
+      <c r="C43" s="84"/>
+      <c r="D43" s="84"/>
+      <c r="E43" s="84"/>
+      <c r="F43" s="84"/>
+      <c r="G43" s="84"/>
+      <c r="H43" s="84"/>
+      <c r="I43" s="84"/>
+      <c r="J43" s="84"/>
+      <c r="K43" s="84"/>
     </row>
     <row r="44" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B44" s="81"/>
-      <c r="C44" s="81"/>
-      <c r="D44" s="81"/>
-      <c r="E44" s="81"/>
-      <c r="F44" s="81"/>
-      <c r="G44" s="81"/>
-      <c r="H44" s="81"/>
-      <c r="I44" s="81"/>
-      <c r="J44" s="81"/>
-      <c r="K44" s="81"/>
+      <c r="B44" s="84"/>
+      <c r="C44" s="84"/>
+      <c r="D44" s="84"/>
+      <c r="E44" s="84"/>
+      <c r="F44" s="84"/>
+      <c r="G44" s="84"/>
+      <c r="H44" s="84"/>
+      <c r="I44" s="84"/>
+      <c r="J44" s="84"/>
+      <c r="K44" s="84"/>
     </row>
     <row r="45" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B45" s="81"/>
-      <c r="C45" s="81"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="81"/>
-      <c r="F45" s="81"/>
-      <c r="G45" s="81"/>
-      <c r="H45" s="81"/>
-      <c r="I45" s="81"/>
-      <c r="J45" s="81"/>
-      <c r="K45" s="81"/>
+      <c r="B45" s="84"/>
+      <c r="C45" s="84"/>
+      <c r="D45" s="84"/>
+      <c r="E45" s="84"/>
+      <c r="F45" s="84"/>
+      <c r="G45" s="84"/>
+      <c r="H45" s="84"/>
+      <c r="I45" s="84"/>
+      <c r="J45" s="84"/>
+      <c r="K45" s="84"/>
     </row>
     <row r="46" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B46" s="81"/>
-      <c r="C46" s="81"/>
-      <c r="D46" s="81"/>
-      <c r="E46" s="81"/>
-      <c r="F46" s="81"/>
-      <c r="G46" s="81"/>
-      <c r="H46" s="81"/>
-      <c r="I46" s="81"/>
-      <c r="J46" s="81"/>
-      <c r="K46" s="81"/>
+      <c r="B46" s="84"/>
+      <c r="C46" s="84"/>
+      <c r="D46" s="84"/>
+      <c r="E46" s="84"/>
+      <c r="F46" s="84"/>
+      <c r="G46" s="84"/>
+      <c r="H46" s="84"/>
+      <c r="I46" s="84"/>
+      <c r="J46" s="84"/>
+      <c r="K46" s="84"/>
     </row>
     <row r="47" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B47" s="81"/>
-      <c r="C47" s="81"/>
-      <c r="D47" s="81"/>
-      <c r="E47" s="81"/>
-      <c r="F47" s="81"/>
-      <c r="G47" s="81"/>
-      <c r="H47" s="81"/>
-      <c r="I47" s="81"/>
-      <c r="J47" s="81"/>
-      <c r="K47" s="81"/>
+      <c r="B47" s="84"/>
+      <c r="C47" s="84"/>
+      <c r="D47" s="84"/>
+      <c r="E47" s="84"/>
+      <c r="F47" s="84"/>
+      <c r="G47" s="84"/>
+      <c r="H47" s="84"/>
+      <c r="I47" s="84"/>
+      <c r="J47" s="84"/>
+      <c r="K47" s="84"/>
     </row>
     <row r="48" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B48" s="81"/>
-      <c r="C48" s="81"/>
-      <c r="D48" s="81"/>
-      <c r="E48" s="81"/>
-      <c r="F48" s="81"/>
-      <c r="G48" s="81"/>
-      <c r="H48" s="81"/>
-      <c r="I48" s="81"/>
-      <c r="J48" s="81"/>
-      <c r="K48" s="81"/>
+      <c r="B48" s="84"/>
+      <c r="C48" s="84"/>
+      <c r="D48" s="84"/>
+      <c r="E48" s="84"/>
+      <c r="F48" s="84"/>
+      <c r="G48" s="84"/>
+      <c r="H48" s="84"/>
+      <c r="I48" s="84"/>
+      <c r="J48" s="84"/>
+      <c r="K48" s="84"/>
     </row>
     <row r="49" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B49" s="81"/>
-      <c r="C49" s="81"/>
-      <c r="D49" s="81"/>
-      <c r="E49" s="81"/>
-      <c r="F49" s="81"/>
-      <c r="G49" s="81"/>
-      <c r="H49" s="81"/>
-      <c r="I49" s="81"/>
-      <c r="J49" s="81"/>
-      <c r="K49" s="81"/>
+      <c r="B49" s="84"/>
+      <c r="C49" s="84"/>
+      <c r="D49" s="84"/>
+      <c r="E49" s="84"/>
+      <c r="F49" s="84"/>
+      <c r="G49" s="84"/>
+      <c r="H49" s="84"/>
+      <c r="I49" s="84"/>
+      <c r="J49" s="84"/>
+      <c r="K49" s="84"/>
     </row>
     <row r="50" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B50" s="81"/>
-      <c r="C50" s="81"/>
-      <c r="D50" s="81"/>
-      <c r="E50" s="81"/>
-      <c r="F50" s="81"/>
-      <c r="G50" s="81"/>
-      <c r="H50" s="81"/>
-      <c r="I50" s="81"/>
-      <c r="J50" s="81"/>
-      <c r="K50" s="81"/>
+      <c r="B50" s="84"/>
+      <c r="C50" s="84"/>
+      <c r="D50" s="84"/>
+      <c r="E50" s="84"/>
+      <c r="F50" s="84"/>
+      <c r="G50" s="84"/>
+      <c r="H50" s="84"/>
+      <c r="I50" s="84"/>
+      <c r="J50" s="84"/>
+      <c r="K50" s="84"/>
     </row>
     <row r="51" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B51" s="81"/>
-      <c r="C51" s="81"/>
-      <c r="D51" s="81"/>
-      <c r="E51" s="81"/>
-      <c r="F51" s="81"/>
-      <c r="G51" s="81"/>
-      <c r="H51" s="81"/>
-      <c r="I51" s="81"/>
-      <c r="J51" s="81"/>
-      <c r="K51" s="81"/>
+      <c r="B51" s="84"/>
+      <c r="C51" s="84"/>
+      <c r="D51" s="84"/>
+      <c r="E51" s="84"/>
+      <c r="F51" s="84"/>
+      <c r="G51" s="84"/>
+      <c r="H51" s="84"/>
+      <c r="I51" s="84"/>
+      <c r="J51" s="84"/>
+      <c r="K51" s="84"/>
     </row>
     <row r="52" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B52" s="81"/>
-      <c r="C52" s="81"/>
-      <c r="D52" s="81"/>
-      <c r="E52" s="81"/>
-      <c r="F52" s="81"/>
-      <c r="G52" s="81"/>
-      <c r="H52" s="81"/>
-      <c r="I52" s="81"/>
-      <c r="J52" s="81"/>
-      <c r="K52" s="81"/>
+      <c r="B52" s="84"/>
+      <c r="C52" s="84"/>
+      <c r="D52" s="84"/>
+      <c r="E52" s="84"/>
+      <c r="F52" s="84"/>
+      <c r="G52" s="84"/>
+      <c r="H52" s="84"/>
+      <c r="I52" s="84"/>
+      <c r="J52" s="84"/>
+      <c r="K52" s="84"/>
     </row>
     <row r="53" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B53" s="81"/>
-      <c r="C53" s="81"/>
-      <c r="D53" s="81"/>
-      <c r="E53" s="81"/>
-      <c r="F53" s="81"/>
-      <c r="G53" s="81"/>
-      <c r="H53" s="81"/>
-      <c r="I53" s="81"/>
-      <c r="J53" s="81"/>
-      <c r="K53" s="81"/>
+      <c r="B53" s="84"/>
+      <c r="C53" s="84"/>
+      <c r="D53" s="84"/>
+      <c r="E53" s="84"/>
+      <c r="F53" s="84"/>
+      <c r="G53" s="84"/>
+      <c r="H53" s="84"/>
+      <c r="I53" s="84"/>
+      <c r="J53" s="84"/>
+      <c r="K53" s="84"/>
     </row>
     <row r="54" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B54" s="81"/>
-      <c r="C54" s="81"/>
-      <c r="D54" s="81"/>
-      <c r="E54" s="81"/>
-      <c r="F54" s="81"/>
-      <c r="G54" s="81"/>
-      <c r="H54" s="81"/>
-      <c r="I54" s="81"/>
-      <c r="J54" s="81"/>
-      <c r="K54" s="81"/>
+      <c r="B54" s="84"/>
+      <c r="C54" s="84"/>
+      <c r="D54" s="84"/>
+      <c r="E54" s="84"/>
+      <c r="F54" s="84"/>
+      <c r="G54" s="84"/>
+      <c r="H54" s="84"/>
+      <c r="I54" s="84"/>
+      <c r="J54" s="84"/>
+      <c r="K54" s="84"/>
     </row>
     <row r="55" spans="2:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B55" s="80" t="s">
+      <c r="B55" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="C55" s="79"/>
-      <c r="D55" s="79"/>
-      <c r="E55" s="79"/>
-      <c r="F55" s="79"/>
-      <c r="G55" s="79"/>
-      <c r="H55" s="79"/>
-      <c r="I55" s="79"/>
-      <c r="J55" s="79"/>
-      <c r="K55" s="79"/>
+      <c r="C55" s="86"/>
+      <c r="D55" s="86"/>
+      <c r="E55" s="86"/>
+      <c r="F55" s="86"/>
+      <c r="G55" s="86"/>
+      <c r="H55" s="86"/>
+      <c r="I55" s="86"/>
+      <c r="J55" s="86"/>
+      <c r="K55" s="86"/>
     </row>
     <row r="56" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B56" s="82" t="s">
+      <c r="B56" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="82"/>
-      <c r="D56" s="82"/>
-      <c r="E56" s="82"/>
-      <c r="F56" s="82"/>
-      <c r="G56" s="82"/>
-      <c r="H56" s="82"/>
-      <c r="I56" s="82"/>
-      <c r="J56" s="82"/>
-      <c r="K56" s="82"/>
+      <c r="C56" s="88"/>
+      <c r="D56" s="88"/>
+      <c r="E56" s="88"/>
+      <c r="F56" s="88"/>
+      <c r="G56" s="88"/>
+      <c r="H56" s="88"/>
+      <c r="I56" s="88"/>
+      <c r="J56" s="88"/>
+      <c r="K56" s="88"/>
     </row>
     <row r="57" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B57" s="82"/>
-      <c r="C57" s="82"/>
-      <c r="D57" s="82"/>
-      <c r="E57" s="82"/>
-      <c r="F57" s="82"/>
-      <c r="G57" s="82"/>
-      <c r="H57" s="82"/>
-      <c r="I57" s="82"/>
-      <c r="J57" s="82"/>
-      <c r="K57" s="82"/>
+      <c r="B57" s="88"/>
+      <c r="C57" s="88"/>
+      <c r="D57" s="88"/>
+      <c r="E57" s="88"/>
+      <c r="F57" s="88"/>
+      <c r="G57" s="88"/>
+      <c r="H57" s="88"/>
+      <c r="I57" s="88"/>
+      <c r="J57" s="88"/>
+      <c r="K57" s="88"/>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B58" s="82"/>
-      <c r="C58" s="82"/>
-      <c r="D58" s="82"/>
-      <c r="E58" s="82"/>
-      <c r="F58" s="82"/>
-      <c r="G58" s="82"/>
-      <c r="H58" s="82"/>
-      <c r="I58" s="82"/>
-      <c r="J58" s="82"/>
-      <c r="K58" s="82"/>
+      <c r="B58" s="88"/>
+      <c r="C58" s="88"/>
+      <c r="D58" s="88"/>
+      <c r="E58" s="88"/>
+      <c r="F58" s="88"/>
+      <c r="G58" s="88"/>
+      <c r="H58" s="88"/>
+      <c r="I58" s="88"/>
+      <c r="J58" s="88"/>
+      <c r="K58" s="88"/>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B59" s="82"/>
-      <c r="C59" s="82"/>
-      <c r="D59" s="82"/>
-      <c r="E59" s="82"/>
-      <c r="F59" s="82"/>
-      <c r="G59" s="82"/>
-      <c r="H59" s="82"/>
-      <c r="I59" s="82"/>
-      <c r="J59" s="82"/>
-      <c r="K59" s="82"/>
+      <c r="B59" s="88"/>
+      <c r="C59" s="88"/>
+      <c r="D59" s="88"/>
+      <c r="E59" s="88"/>
+      <c r="F59" s="88"/>
+      <c r="G59" s="88"/>
+      <c r="H59" s="88"/>
+      <c r="I59" s="88"/>
+      <c r="J59" s="88"/>
+      <c r="K59" s="88"/>
     </row>
     <row r="61" spans="2:11" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B61" s="13"/>
@@ -2616,77 +2616,77 @@
       <c r="C65" s="28"/>
     </row>
     <row r="66" spans="2:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="B66" s="85" t="s">
+      <c r="B66" s="70" t="s">
         <v>28</v>
       </c>
       <c r="C66" s="55"/>
       <c r="D66" s="36"/>
-      <c r="F66" s="84" t="s">
+      <c r="F66" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="G66" s="84"/>
-      <c r="H66" s="84"/>
-      <c r="I66" s="84"/>
-      <c r="J66" s="84"/>
-      <c r="K66" s="84"/>
+      <c r="G66" s="87"/>
+      <c r="H66" s="87"/>
+      <c r="I66" s="87"/>
+      <c r="J66" s="87"/>
+      <c r="K66" s="87"/>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B70" s="86" t="s">
+      <c r="B70" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="C70" s="83"/>
-      <c r="G70" s="87" t="s">
+      <c r="C70" s="81"/>
+      <c r="G70" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="H70" s="88"/>
-      <c r="I70" s="88"/>
-      <c r="J70" s="88"/>
-      <c r="K70" s="88"/>
+      <c r="H70" s="83"/>
+      <c r="I70" s="83"/>
+      <c r="J70" s="83"/>
+      <c r="K70" s="83"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B71" s="83"/>
-      <c r="C71" s="83"/>
-      <c r="G71" s="88"/>
-      <c r="H71" s="88"/>
-      <c r="I71" s="88"/>
-      <c r="J71" s="88"/>
-      <c r="K71" s="88"/>
+      <c r="B71" s="81"/>
+      <c r="C71" s="81"/>
+      <c r="G71" s="83"/>
+      <c r="H71" s="83"/>
+      <c r="I71" s="83"/>
+      <c r="J71" s="83"/>
+      <c r="K71" s="83"/>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B72" s="83"/>
-      <c r="C72" s="83"/>
-      <c r="G72" s="88"/>
-      <c r="H72" s="88"/>
-      <c r="I72" s="88"/>
-      <c r="J72" s="88"/>
-      <c r="K72" s="88"/>
+      <c r="B72" s="81"/>
+      <c r="C72" s="81"/>
+      <c r="G72" s="83"/>
+      <c r="H72" s="83"/>
+      <c r="I72" s="83"/>
+      <c r="J72" s="83"/>
+      <c r="K72" s="83"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B73" s="83"/>
-      <c r="C73" s="83"/>
-      <c r="G73" s="88"/>
-      <c r="H73" s="88"/>
-      <c r="I73" s="88"/>
-      <c r="J73" s="88"/>
-      <c r="K73" s="88"/>
+      <c r="B73" s="81"/>
+      <c r="C73" s="81"/>
+      <c r="G73" s="83"/>
+      <c r="H73" s="83"/>
+      <c r="I73" s="83"/>
+      <c r="J73" s="83"/>
+      <c r="K73" s="83"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B74" s="83"/>
-      <c r="C74" s="83"/>
-      <c r="G74" s="88"/>
-      <c r="H74" s="88"/>
-      <c r="I74" s="88"/>
-      <c r="J74" s="88"/>
-      <c r="K74" s="88"/>
+      <c r="B74" s="81"/>
+      <c r="C74" s="81"/>
+      <c r="G74" s="83"/>
+      <c r="H74" s="83"/>
+      <c r="I74" s="83"/>
+      <c r="J74" s="83"/>
+      <c r="K74" s="83"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B75" s="83"/>
-      <c r="C75" s="83"/>
-      <c r="G75" s="88"/>
-      <c r="H75" s="88"/>
-      <c r="I75" s="88"/>
-      <c r="J75" s="88"/>
-      <c r="K75" s="88"/>
+      <c r="B75" s="81"/>
+      <c r="C75" s="81"/>
+      <c r="G75" s="83"/>
+      <c r="H75" s="83"/>
+      <c r="I75" s="83"/>
+      <c r="J75" s="83"/>
+      <c r="K75" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -2740,7 +2740,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="46" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="48" orientation="portrait" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddHeader>&amp;C&amp;"System Font,Normale"&amp;10&amp;K000000cliente</oddHeader>
   </headerFooter>
@@ -2764,7 +2764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E2739A-1A6E-2F4E-AE98-2EAEF954239A}">
   <dimension ref="C1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modifica temoplate riparazione aggiunta dati prodotti_aggiuntivi in excel fix checkprodottiaggiuntivi
</commit_message>
<xml_diff>
--- a/src/assets/template_riparazione.xlsx
+++ b/src/assets/template_riparazione.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr filterPrivacy="1" codeName="Questa_cartella_di_lavoro"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CB72C2-F6CD-A54F-955D-4573D9BAE2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF1B06C-4D5E-1F45-9521-0727CF36F82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -164,13 +164,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="&quot;€&quot;\ #,##0.00"/>
     <numFmt numFmtId="167" formatCode="\-"/>
+    <numFmt numFmtId="168" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="47" x14ac:knownFonts="1">
     <font>
@@ -1171,15 +1172,6 @@
     <xf numFmtId="0" fontId="33" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="35" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="30" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="30" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
@@ -1315,6 +1307,15 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="30" fillId="35" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -1966,8 +1967,8 @@
   </sheetPr>
   <dimension ref="B1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B70" sqref="B1:K75"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2010,7 +2011,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="34"/>
-      <c r="D4" s="61"/>
+      <c r="D4" s="58"/>
       <c r="E4" s="32"/>
       <c r="F4" s="32" t="s">
         <v>15</v>
@@ -2023,8 +2024,8 @@
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="21"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="73"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="70"/>
     </row>
     <row r="6" spans="2:11" s="9" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="34" t="s">
@@ -2032,33 +2033,33 @@
       </c>
       <c r="C6" s="34"/>
       <c r="D6" s="21"/>
-      <c r="F6" s="73"/>
+      <c r="F6" s="70"/>
     </row>
     <row r="7" spans="2:11" s="9" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="34"/>
-      <c r="D7" s="60"/>
+      <c r="D7" s="57"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="2:11" s="9" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="69"/>
-      <c r="D8" s="60"/>
-      <c r="F8" s="64"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="57"/>
+      <c r="F8" s="61"/>
     </row>
     <row r="9" spans="2:11" s="3" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="D9" s="22"/>
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="2:11" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="78" t="s">
+      <c r="B10" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="79"/>
+      <c r="C10" s="76"/>
       <c r="D10" s="38" t="s">
         <v>9</v>
       </c>
@@ -2070,36 +2071,36 @@
       </c>
     </row>
     <row r="11" spans="2:11" s="4" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="74"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="40"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="86"/>
       <c r="I11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="K11" s="35"/>
     </row>
     <row r="12" spans="2:11" s="4" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="74"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="41"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="87"/>
     </row>
     <row r="13" spans="2:11" s="4" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="74"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="40"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="86"/>
     </row>
     <row r="14" spans="2:11" s="4" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="76"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="42"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="88"/>
     </row>
     <row r="15" spans="2:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F15" s="14"/>
@@ -2108,7 +2109,7 @@
     <row r="16" spans="2:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="63"/>
+      <c r="D16" s="60"/>
       <c r="E16" s="29" t="s">
         <v>0</v>
       </c>
@@ -2118,11 +2119,11 @@
       </c>
     </row>
     <row r="17" spans="2:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="49"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="46"/>
       <c r="E17" s="29" t="s">
         <v>1</v>
       </c>
@@ -2140,11 +2141,11 @@
       <c r="F18" s="31"/>
     </row>
     <row r="19" spans="2:11" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="51" t="s">
+      <c r="C19" s="40"/>
+      <c r="D19" s="48" t="s">
         <v>18</v>
       </c>
       <c r="E19" s="29" t="s">
@@ -2167,17 +2168,17 @@
       </c>
     </row>
     <row r="21" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="72" t="s">
+      <c r="B21" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="69"/>
     </row>
     <row r="22" spans="2:11" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="7"/>
@@ -2188,8 +2189,8 @@
     <row r="23" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
-      <c r="D23" s="56"/>
-      <c r="F23" s="71"/>
+      <c r="D23" s="53"/>
+      <c r="F23" s="68"/>
     </row>
     <row r="24" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="12" t="str">
@@ -2197,9 +2198,9 @@
         <v>Nome Cognome:</v>
       </c>
       <c r="C24" s="12"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="71"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="68"/>
     </row>
     <row r="25" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="12" t="str">
@@ -2207,7 +2208,7 @@
         <v>Indirizzo:</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="60"/>
+      <c r="D25" s="57"/>
     </row>
     <row r="26" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="12" t="str">
@@ -2216,10 +2217,10 @@
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="26"/>
-      <c r="E26" s="54" t="s">
+      <c r="E26" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="48">
+      <c r="F26" s="45">
         <f>F18</f>
         <v>0</v>
       </c>
@@ -2231,10 +2232,10 @@
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="26"/>
-      <c r="E27" s="54" t="s">
+      <c r="E27" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="48"/>
+      <c r="F27" s="45"/>
     </row>
     <row r="28" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="12"/>
@@ -2252,358 +2253,358 @@
       <c r="D30" s="26"/>
     </row>
     <row r="31" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="84" t="s">
+      <c r="B31" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="84"/>
-      <c r="D31" s="84"/>
-      <c r="E31" s="84"/>
-      <c r="F31" s="84"/>
-      <c r="G31" s="84"/>
-      <c r="H31" s="84"/>
-      <c r="I31" s="84"/>
-      <c r="J31" s="84"/>
-      <c r="K31" s="84"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="81"/>
+      <c r="F31" s="81"/>
+      <c r="G31" s="81"/>
+      <c r="H31" s="81"/>
+      <c r="I31" s="81"/>
+      <c r="J31" s="81"/>
+      <c r="K31" s="81"/>
     </row>
     <row r="32" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B32" s="84"/>
-      <c r="C32" s="84"/>
-      <c r="D32" s="84"/>
-      <c r="E32" s="84"/>
-      <c r="F32" s="84"/>
-      <c r="G32" s="84"/>
-      <c r="H32" s="84"/>
-      <c r="I32" s="84"/>
-      <c r="J32" s="84"/>
-      <c r="K32" s="84"/>
+      <c r="B32" s="81"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="81"/>
+      <c r="E32" s="81"/>
+      <c r="F32" s="81"/>
+      <c r="G32" s="81"/>
+      <c r="H32" s="81"/>
+      <c r="I32" s="81"/>
+      <c r="J32" s="81"/>
+      <c r="K32" s="81"/>
     </row>
     <row r="33" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="84"/>
-      <c r="C33" s="84"/>
-      <c r="D33" s="84"/>
-      <c r="E33" s="84"/>
-      <c r="F33" s="84"/>
-      <c r="G33" s="84"/>
-      <c r="H33" s="84"/>
-      <c r="I33" s="84"/>
-      <c r="J33" s="84"/>
-      <c r="K33" s="84"/>
+      <c r="B33" s="81"/>
+      <c r="C33" s="81"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="81"/>
+      <c r="F33" s="81"/>
+      <c r="G33" s="81"/>
+      <c r="H33" s="81"/>
+      <c r="I33" s="81"/>
+      <c r="J33" s="81"/>
+      <c r="K33" s="81"/>
     </row>
     <row r="34" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="84"/>
-      <c r="C34" s="84"/>
-      <c r="D34" s="84"/>
-      <c r="E34" s="84"/>
-      <c r="F34" s="84"/>
-      <c r="G34" s="84"/>
-      <c r="H34" s="84"/>
-      <c r="I34" s="84"/>
-      <c r="J34" s="84"/>
-      <c r="K34" s="84"/>
+      <c r="B34" s="81"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="81"/>
+      <c r="G34" s="81"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="81"/>
+      <c r="J34" s="81"/>
+      <c r="K34" s="81"/>
     </row>
     <row r="35" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B35" s="84"/>
-      <c r="C35" s="84"/>
-      <c r="D35" s="84"/>
-      <c r="E35" s="84"/>
-      <c r="F35" s="84"/>
-      <c r="G35" s="84"/>
-      <c r="H35" s="84"/>
-      <c r="I35" s="84"/>
-      <c r="J35" s="84"/>
-      <c r="K35" s="84"/>
+      <c r="B35" s="81"/>
+      <c r="C35" s="81"/>
+      <c r="D35" s="81"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="81"/>
+      <c r="G35" s="81"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="81"/>
+      <c r="J35" s="81"/>
+      <c r="K35" s="81"/>
     </row>
     <row r="36" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="84"/>
-      <c r="C36" s="84"/>
-      <c r="D36" s="84"/>
-      <c r="E36" s="84"/>
-      <c r="F36" s="84"/>
-      <c r="G36" s="84"/>
-      <c r="H36" s="84"/>
-      <c r="I36" s="84"/>
-      <c r="J36" s="84"/>
-      <c r="K36" s="84"/>
+      <c r="B36" s="81"/>
+      <c r="C36" s="81"/>
+      <c r="D36" s="81"/>
+      <c r="E36" s="81"/>
+      <c r="F36" s="81"/>
+      <c r="G36" s="81"/>
+      <c r="H36" s="81"/>
+      <c r="I36" s="81"/>
+      <c r="J36" s="81"/>
+      <c r="K36" s="81"/>
     </row>
     <row r="37" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="84"/>
-      <c r="C37" s="84"/>
-      <c r="D37" s="84"/>
-      <c r="E37" s="84"/>
-      <c r="F37" s="84"/>
-      <c r="G37" s="84"/>
-      <c r="H37" s="84"/>
-      <c r="I37" s="84"/>
-      <c r="J37" s="84"/>
-      <c r="K37" s="84"/>
+      <c r="B37" s="81"/>
+      <c r="C37" s="81"/>
+      <c r="D37" s="81"/>
+      <c r="E37" s="81"/>
+      <c r="F37" s="81"/>
+      <c r="G37" s="81"/>
+      <c r="H37" s="81"/>
+      <c r="I37" s="81"/>
+      <c r="J37" s="81"/>
+      <c r="K37" s="81"/>
     </row>
     <row r="38" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B38" s="84"/>
-      <c r="C38" s="84"/>
-      <c r="D38" s="84"/>
-      <c r="E38" s="84"/>
-      <c r="F38" s="84"/>
-      <c r="G38" s="84"/>
-      <c r="H38" s="84"/>
-      <c r="I38" s="84"/>
-      <c r="J38" s="84"/>
-      <c r="K38" s="84"/>
+      <c r="B38" s="81"/>
+      <c r="C38" s="81"/>
+      <c r="D38" s="81"/>
+      <c r="E38" s="81"/>
+      <c r="F38" s="81"/>
+      <c r="G38" s="81"/>
+      <c r="H38" s="81"/>
+      <c r="I38" s="81"/>
+      <c r="J38" s="81"/>
+      <c r="K38" s="81"/>
     </row>
     <row r="39" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B39" s="84"/>
-      <c r="C39" s="84"/>
-      <c r="D39" s="84"/>
-      <c r="E39" s="84"/>
-      <c r="F39" s="84"/>
-      <c r="G39" s="84"/>
-      <c r="H39" s="84"/>
-      <c r="I39" s="84"/>
-      <c r="J39" s="84"/>
-      <c r="K39" s="84"/>
+      <c r="B39" s="81"/>
+      <c r="C39" s="81"/>
+      <c r="D39" s="81"/>
+      <c r="E39" s="81"/>
+      <c r="F39" s="81"/>
+      <c r="G39" s="81"/>
+      <c r="H39" s="81"/>
+      <c r="I39" s="81"/>
+      <c r="J39" s="81"/>
+      <c r="K39" s="81"/>
     </row>
     <row r="40" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B40" s="84"/>
-      <c r="C40" s="84"/>
-      <c r="D40" s="84"/>
-      <c r="E40" s="84"/>
-      <c r="F40" s="84"/>
-      <c r="G40" s="84"/>
-      <c r="H40" s="84"/>
-      <c r="I40" s="84"/>
-      <c r="J40" s="84"/>
-      <c r="K40" s="84"/>
+      <c r="B40" s="81"/>
+      <c r="C40" s="81"/>
+      <c r="D40" s="81"/>
+      <c r="E40" s="81"/>
+      <c r="F40" s="81"/>
+      <c r="G40" s="81"/>
+      <c r="H40" s="81"/>
+      <c r="I40" s="81"/>
+      <c r="J40" s="81"/>
+      <c r="K40" s="81"/>
     </row>
     <row r="41" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B41" s="84"/>
-      <c r="C41" s="84"/>
-      <c r="D41" s="84"/>
-      <c r="E41" s="84"/>
-      <c r="F41" s="84"/>
-      <c r="G41" s="84"/>
-      <c r="H41" s="84"/>
-      <c r="I41" s="84"/>
-      <c r="J41" s="84"/>
-      <c r="K41" s="84"/>
+      <c r="B41" s="81"/>
+      <c r="C41" s="81"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="81"/>
+      <c r="F41" s="81"/>
+      <c r="G41" s="81"/>
+      <c r="H41" s="81"/>
+      <c r="I41" s="81"/>
+      <c r="J41" s="81"/>
+      <c r="K41" s="81"/>
     </row>
     <row r="42" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B42" s="84"/>
-      <c r="C42" s="84"/>
-      <c r="D42" s="84"/>
-      <c r="E42" s="84"/>
-      <c r="F42" s="84"/>
-      <c r="G42" s="84"/>
-      <c r="H42" s="84"/>
-      <c r="I42" s="84"/>
-      <c r="J42" s="84"/>
-      <c r="K42" s="84"/>
+      <c r="B42" s="81"/>
+      <c r="C42" s="81"/>
+      <c r="D42" s="81"/>
+      <c r="E42" s="81"/>
+      <c r="F42" s="81"/>
+      <c r="G42" s="81"/>
+      <c r="H42" s="81"/>
+      <c r="I42" s="81"/>
+      <c r="J42" s="81"/>
+      <c r="K42" s="81"/>
     </row>
     <row r="43" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B43" s="84"/>
-      <c r="C43" s="84"/>
-      <c r="D43" s="84"/>
-      <c r="E43" s="84"/>
-      <c r="F43" s="84"/>
-      <c r="G43" s="84"/>
-      <c r="H43" s="84"/>
-      <c r="I43" s="84"/>
-      <c r="J43" s="84"/>
-      <c r="K43" s="84"/>
+      <c r="B43" s="81"/>
+      <c r="C43" s="81"/>
+      <c r="D43" s="81"/>
+      <c r="E43" s="81"/>
+      <c r="F43" s="81"/>
+      <c r="G43" s="81"/>
+      <c r="H43" s="81"/>
+      <c r="I43" s="81"/>
+      <c r="J43" s="81"/>
+      <c r="K43" s="81"/>
     </row>
     <row r="44" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B44" s="84"/>
-      <c r="C44" s="84"/>
-      <c r="D44" s="84"/>
-      <c r="E44" s="84"/>
-      <c r="F44" s="84"/>
-      <c r="G44" s="84"/>
-      <c r="H44" s="84"/>
-      <c r="I44" s="84"/>
-      <c r="J44" s="84"/>
-      <c r="K44" s="84"/>
+      <c r="B44" s="81"/>
+      <c r="C44" s="81"/>
+      <c r="D44" s="81"/>
+      <c r="E44" s="81"/>
+      <c r="F44" s="81"/>
+      <c r="G44" s="81"/>
+      <c r="H44" s="81"/>
+      <c r="I44" s="81"/>
+      <c r="J44" s="81"/>
+      <c r="K44" s="81"/>
     </row>
     <row r="45" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B45" s="84"/>
-      <c r="C45" s="84"/>
-      <c r="D45" s="84"/>
-      <c r="E45" s="84"/>
-      <c r="F45" s="84"/>
-      <c r="G45" s="84"/>
-      <c r="H45" s="84"/>
-      <c r="I45" s="84"/>
-      <c r="J45" s="84"/>
-      <c r="K45" s="84"/>
+      <c r="B45" s="81"/>
+      <c r="C45" s="81"/>
+      <c r="D45" s="81"/>
+      <c r="E45" s="81"/>
+      <c r="F45" s="81"/>
+      <c r="G45" s="81"/>
+      <c r="H45" s="81"/>
+      <c r="I45" s="81"/>
+      <c r="J45" s="81"/>
+      <c r="K45" s="81"/>
     </row>
     <row r="46" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B46" s="84"/>
-      <c r="C46" s="84"/>
-      <c r="D46" s="84"/>
-      <c r="E46" s="84"/>
-      <c r="F46" s="84"/>
-      <c r="G46" s="84"/>
-      <c r="H46" s="84"/>
-      <c r="I46" s="84"/>
-      <c r="J46" s="84"/>
-      <c r="K46" s="84"/>
+      <c r="B46" s="81"/>
+      <c r="C46" s="81"/>
+      <c r="D46" s="81"/>
+      <c r="E46" s="81"/>
+      <c r="F46" s="81"/>
+      <c r="G46" s="81"/>
+      <c r="H46" s="81"/>
+      <c r="I46" s="81"/>
+      <c r="J46" s="81"/>
+      <c r="K46" s="81"/>
     </row>
     <row r="47" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B47" s="84"/>
-      <c r="C47" s="84"/>
-      <c r="D47" s="84"/>
-      <c r="E47" s="84"/>
-      <c r="F47" s="84"/>
-      <c r="G47" s="84"/>
-      <c r="H47" s="84"/>
-      <c r="I47" s="84"/>
-      <c r="J47" s="84"/>
-      <c r="K47" s="84"/>
+      <c r="B47" s="81"/>
+      <c r="C47" s="81"/>
+      <c r="D47" s="81"/>
+      <c r="E47" s="81"/>
+      <c r="F47" s="81"/>
+      <c r="G47" s="81"/>
+      <c r="H47" s="81"/>
+      <c r="I47" s="81"/>
+      <c r="J47" s="81"/>
+      <c r="K47" s="81"/>
     </row>
     <row r="48" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B48" s="84"/>
-      <c r="C48" s="84"/>
-      <c r="D48" s="84"/>
-      <c r="E48" s="84"/>
-      <c r="F48" s="84"/>
-      <c r="G48" s="84"/>
-      <c r="H48" s="84"/>
-      <c r="I48" s="84"/>
-      <c r="J48" s="84"/>
-      <c r="K48" s="84"/>
+      <c r="B48" s="81"/>
+      <c r="C48" s="81"/>
+      <c r="D48" s="81"/>
+      <c r="E48" s="81"/>
+      <c r="F48" s="81"/>
+      <c r="G48" s="81"/>
+      <c r="H48" s="81"/>
+      <c r="I48" s="81"/>
+      <c r="J48" s="81"/>
+      <c r="K48" s="81"/>
     </row>
     <row r="49" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B49" s="84"/>
-      <c r="C49" s="84"/>
-      <c r="D49" s="84"/>
-      <c r="E49" s="84"/>
-      <c r="F49" s="84"/>
-      <c r="G49" s="84"/>
-      <c r="H49" s="84"/>
-      <c r="I49" s="84"/>
-      <c r="J49" s="84"/>
-      <c r="K49" s="84"/>
+      <c r="B49" s="81"/>
+      <c r="C49" s="81"/>
+      <c r="D49" s="81"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="81"/>
+      <c r="G49" s="81"/>
+      <c r="H49" s="81"/>
+      <c r="I49" s="81"/>
+      <c r="J49" s="81"/>
+      <c r="K49" s="81"/>
     </row>
     <row r="50" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B50" s="84"/>
-      <c r="C50" s="84"/>
-      <c r="D50" s="84"/>
-      <c r="E50" s="84"/>
-      <c r="F50" s="84"/>
-      <c r="G50" s="84"/>
-      <c r="H50" s="84"/>
-      <c r="I50" s="84"/>
-      <c r="J50" s="84"/>
-      <c r="K50" s="84"/>
+      <c r="B50" s="81"/>
+      <c r="C50" s="81"/>
+      <c r="D50" s="81"/>
+      <c r="E50" s="81"/>
+      <c r="F50" s="81"/>
+      <c r="G50" s="81"/>
+      <c r="H50" s="81"/>
+      <c r="I50" s="81"/>
+      <c r="J50" s="81"/>
+      <c r="K50" s="81"/>
     </row>
     <row r="51" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B51" s="84"/>
-      <c r="C51" s="84"/>
-      <c r="D51" s="84"/>
-      <c r="E51" s="84"/>
-      <c r="F51" s="84"/>
-      <c r="G51" s="84"/>
-      <c r="H51" s="84"/>
-      <c r="I51" s="84"/>
-      <c r="J51" s="84"/>
-      <c r="K51" s="84"/>
+      <c r="B51" s="81"/>
+      <c r="C51" s="81"/>
+      <c r="D51" s="81"/>
+      <c r="E51" s="81"/>
+      <c r="F51" s="81"/>
+      <c r="G51" s="81"/>
+      <c r="H51" s="81"/>
+      <c r="I51" s="81"/>
+      <c r="J51" s="81"/>
+      <c r="K51" s="81"/>
     </row>
     <row r="52" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B52" s="84"/>
-      <c r="C52" s="84"/>
-      <c r="D52" s="84"/>
-      <c r="E52" s="84"/>
-      <c r="F52" s="84"/>
-      <c r="G52" s="84"/>
-      <c r="H52" s="84"/>
-      <c r="I52" s="84"/>
-      <c r="J52" s="84"/>
-      <c r="K52" s="84"/>
+      <c r="B52" s="81"/>
+      <c r="C52" s="81"/>
+      <c r="D52" s="81"/>
+      <c r="E52" s="81"/>
+      <c r="F52" s="81"/>
+      <c r="G52" s="81"/>
+      <c r="H52" s="81"/>
+      <c r="I52" s="81"/>
+      <c r="J52" s="81"/>
+      <c r="K52" s="81"/>
     </row>
     <row r="53" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B53" s="84"/>
-      <c r="C53" s="84"/>
-      <c r="D53" s="84"/>
-      <c r="E53" s="84"/>
-      <c r="F53" s="84"/>
-      <c r="G53" s="84"/>
-      <c r="H53" s="84"/>
-      <c r="I53" s="84"/>
-      <c r="J53" s="84"/>
-      <c r="K53" s="84"/>
+      <c r="B53" s="81"/>
+      <c r="C53" s="81"/>
+      <c r="D53" s="81"/>
+      <c r="E53" s="81"/>
+      <c r="F53" s="81"/>
+      <c r="G53" s="81"/>
+      <c r="H53" s="81"/>
+      <c r="I53" s="81"/>
+      <c r="J53" s="81"/>
+      <c r="K53" s="81"/>
     </row>
     <row r="54" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B54" s="84"/>
-      <c r="C54" s="84"/>
-      <c r="D54" s="84"/>
-      <c r="E54" s="84"/>
-      <c r="F54" s="84"/>
-      <c r="G54" s="84"/>
-      <c r="H54" s="84"/>
-      <c r="I54" s="84"/>
-      <c r="J54" s="84"/>
-      <c r="K54" s="84"/>
+      <c r="B54" s="81"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="81"/>
+      <c r="E54" s="81"/>
+      <c r="F54" s="81"/>
+      <c r="G54" s="81"/>
+      <c r="H54" s="81"/>
+      <c r="I54" s="81"/>
+      <c r="J54" s="81"/>
+      <c r="K54" s="81"/>
     </row>
     <row r="55" spans="2:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B55" s="85" t="s">
+      <c r="B55" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="C55" s="86"/>
-      <c r="D55" s="86"/>
-      <c r="E55" s="86"/>
-      <c r="F55" s="86"/>
-      <c r="G55" s="86"/>
-      <c r="H55" s="86"/>
-      <c r="I55" s="86"/>
-      <c r="J55" s="86"/>
-      <c r="K55" s="86"/>
+      <c r="C55" s="83"/>
+      <c r="D55" s="83"/>
+      <c r="E55" s="83"/>
+      <c r="F55" s="83"/>
+      <c r="G55" s="83"/>
+      <c r="H55" s="83"/>
+      <c r="I55" s="83"/>
+      <c r="J55" s="83"/>
+      <c r="K55" s="83"/>
     </row>
     <row r="56" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B56" s="88" t="s">
+      <c r="B56" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="88"/>
-      <c r="D56" s="88"/>
-      <c r="E56" s="88"/>
-      <c r="F56" s="88"/>
-      <c r="G56" s="88"/>
-      <c r="H56" s="88"/>
-      <c r="I56" s="88"/>
-      <c r="J56" s="88"/>
-      <c r="K56" s="88"/>
+      <c r="C56" s="85"/>
+      <c r="D56" s="85"/>
+      <c r="E56" s="85"/>
+      <c r="F56" s="85"/>
+      <c r="G56" s="85"/>
+      <c r="H56" s="85"/>
+      <c r="I56" s="85"/>
+      <c r="J56" s="85"/>
+      <c r="K56" s="85"/>
     </row>
     <row r="57" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B57" s="88"/>
-      <c r="C57" s="88"/>
-      <c r="D57" s="88"/>
-      <c r="E57" s="88"/>
-      <c r="F57" s="88"/>
-      <c r="G57" s="88"/>
-      <c r="H57" s="88"/>
-      <c r="I57" s="88"/>
-      <c r="J57" s="88"/>
-      <c r="K57" s="88"/>
+      <c r="B57" s="85"/>
+      <c r="C57" s="85"/>
+      <c r="D57" s="85"/>
+      <c r="E57" s="85"/>
+      <c r="F57" s="85"/>
+      <c r="G57" s="85"/>
+      <c r="H57" s="85"/>
+      <c r="I57" s="85"/>
+      <c r="J57" s="85"/>
+      <c r="K57" s="85"/>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B58" s="88"/>
-      <c r="C58" s="88"/>
-      <c r="D58" s="88"/>
-      <c r="E58" s="88"/>
-      <c r="F58" s="88"/>
-      <c r="G58" s="88"/>
-      <c r="H58" s="88"/>
-      <c r="I58" s="88"/>
-      <c r="J58" s="88"/>
-      <c r="K58" s="88"/>
+      <c r="B58" s="85"/>
+      <c r="C58" s="85"/>
+      <c r="D58" s="85"/>
+      <c r="E58" s="85"/>
+      <c r="F58" s="85"/>
+      <c r="G58" s="85"/>
+      <c r="H58" s="85"/>
+      <c r="I58" s="85"/>
+      <c r="J58" s="85"/>
+      <c r="K58" s="85"/>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B59" s="88"/>
-      <c r="C59" s="88"/>
-      <c r="D59" s="88"/>
-      <c r="E59" s="88"/>
-      <c r="F59" s="88"/>
-      <c r="G59" s="88"/>
-      <c r="H59" s="88"/>
-      <c r="I59" s="88"/>
-      <c r="J59" s="88"/>
-      <c r="K59" s="88"/>
+      <c r="B59" s="85"/>
+      <c r="C59" s="85"/>
+      <c r="D59" s="85"/>
+      <c r="E59" s="85"/>
+      <c r="F59" s="85"/>
+      <c r="G59" s="85"/>
+      <c r="H59" s="85"/>
+      <c r="I59" s="85"/>
+      <c r="J59" s="85"/>
+      <c r="K59" s="85"/>
     </row>
     <row r="61" spans="2:11" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B61" s="13"/>
@@ -2616,77 +2617,77 @@
       <c r="C65" s="28"/>
     </row>
     <row r="66" spans="2:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="B66" s="70" t="s">
+      <c r="B66" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C66" s="55"/>
+      <c r="C66" s="52"/>
       <c r="D66" s="36"/>
-      <c r="F66" s="87" t="s">
+      <c r="F66" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="G66" s="87"/>
-      <c r="H66" s="87"/>
-      <c r="I66" s="87"/>
-      <c r="J66" s="87"/>
-      <c r="K66" s="87"/>
+      <c r="G66" s="84"/>
+      <c r="H66" s="84"/>
+      <c r="I66" s="84"/>
+      <c r="J66" s="84"/>
+      <c r="K66" s="84"/>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B70" s="80" t="s">
+      <c r="B70" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="C70" s="81"/>
-      <c r="G70" s="82" t="s">
+      <c r="C70" s="78"/>
+      <c r="G70" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="H70" s="83"/>
-      <c r="I70" s="83"/>
-      <c r="J70" s="83"/>
-      <c r="K70" s="83"/>
+      <c r="H70" s="80"/>
+      <c r="I70" s="80"/>
+      <c r="J70" s="80"/>
+      <c r="K70" s="80"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B71" s="81"/>
-      <c r="C71" s="81"/>
-      <c r="G71" s="83"/>
-      <c r="H71" s="83"/>
-      <c r="I71" s="83"/>
-      <c r="J71" s="83"/>
-      <c r="K71" s="83"/>
+      <c r="B71" s="78"/>
+      <c r="C71" s="78"/>
+      <c r="G71" s="80"/>
+      <c r="H71" s="80"/>
+      <c r="I71" s="80"/>
+      <c r="J71" s="80"/>
+      <c r="K71" s="80"/>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B72" s="81"/>
-      <c r="C72" s="81"/>
-      <c r="G72" s="83"/>
-      <c r="H72" s="83"/>
-      <c r="I72" s="83"/>
-      <c r="J72" s="83"/>
-      <c r="K72" s="83"/>
+      <c r="B72" s="78"/>
+      <c r="C72" s="78"/>
+      <c r="G72" s="80"/>
+      <c r="H72" s="80"/>
+      <c r="I72" s="80"/>
+      <c r="J72" s="80"/>
+      <c r="K72" s="80"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B73" s="81"/>
-      <c r="C73" s="81"/>
-      <c r="G73" s="83"/>
-      <c r="H73" s="83"/>
-      <c r="I73" s="83"/>
-      <c r="J73" s="83"/>
-      <c r="K73" s="83"/>
+      <c r="B73" s="78"/>
+      <c r="C73" s="78"/>
+      <c r="G73" s="80"/>
+      <c r="H73" s="80"/>
+      <c r="I73" s="80"/>
+      <c r="J73" s="80"/>
+      <c r="K73" s="80"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B74" s="81"/>
-      <c r="C74" s="81"/>
-      <c r="G74" s="83"/>
-      <c r="H74" s="83"/>
-      <c r="I74" s="83"/>
-      <c r="J74" s="83"/>
-      <c r="K74" s="83"/>
+      <c r="B74" s="78"/>
+      <c r="C74" s="78"/>
+      <c r="G74" s="80"/>
+      <c r="H74" s="80"/>
+      <c r="I74" s="80"/>
+      <c r="J74" s="80"/>
+      <c r="K74" s="80"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B75" s="81"/>
-      <c r="C75" s="81"/>
-      <c r="G75" s="83"/>
-      <c r="H75" s="83"/>
-      <c r="I75" s="83"/>
-      <c r="J75" s="83"/>
-      <c r="K75" s="83"/>
+      <c r="B75" s="78"/>
+      <c r="C75" s="78"/>
+      <c r="G75" s="80"/>
+      <c r="H75" s="80"/>
+      <c r="I75" s="80"/>
+      <c r="J75" s="80"/>
+      <c r="K75" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -2770,21 +2771,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="22.6640625" style="57" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="54" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="54" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="3:3" x14ac:dyDescent="0.15">
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="55" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="3:3" x14ac:dyDescent="0.15">
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="56" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>